<commit_message>
starting more complex networks
</commit_message>
<xml_diff>
--- a/fixed_point_methods/inv_demand.xlsx
+++ b/fixed_point_methods/inv_demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasfuentes/ASL/ICU/fixed_point_methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A03EDC1-9632-404E-B0CD-5FF96F0A09D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB14B579-0DB3-4F43-B7D1-4C6C8BA34933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{3EBCDA5C-E193-F340-AD4B-1D4D715CF179}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,10 +435,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>